<commit_message>
updated jupyter notebook and some other stuff
</commit_message>
<xml_diff>
--- a/xls/subject_author_analysis_repaired.xlsx
+++ b/xls/subject_author_analysis_repaired.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="all_authors" sheetId="1" r:id="rId1"/>
@@ -550,7 +550,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -893,8 +892,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="343326208"/>
-        <c:axId val="343330688"/>
+        <c:axId val="266612480"/>
+        <c:axId val="265774176"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -987,7 +986,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="343326208"/>
+        <c:axId val="266612480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,7 +1029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343330688"/>
+        <c:crossAx val="265774176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1038,7 +1037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343330688"/>
+        <c:axId val="265774176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,7 +1088,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343326208"/>
+        <c:crossAx val="266612480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1103,7 +1102,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1215,7 +1213,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1331,11 +1328,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="343323968"/>
-        <c:axId val="343328448"/>
+        <c:axId val="393527920"/>
+        <c:axId val="393528480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="343323968"/>
+        <c:axId val="393527920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,7 +1375,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343328448"/>
+        <c:crossAx val="393528480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1386,7 +1383,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343328448"/>
+        <c:axId val="393528480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1437,7 +1434,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343323968"/>
+        <c:crossAx val="393527920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1531,7 +1528,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1621,11 +1617,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="343332928"/>
-        <c:axId val="343334608"/>
+        <c:axId val="393530720"/>
+        <c:axId val="393531280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="343332928"/>
+        <c:axId val="393530720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1668,7 +1664,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343334608"/>
+        <c:crossAx val="393531280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1676,7 +1672,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343334608"/>
+        <c:axId val="393531280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1723,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343332928"/>
+        <c:crossAx val="393530720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1821,7 +1817,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1990,11 +1985,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="343330128"/>
-        <c:axId val="343324528"/>
+        <c:axId val="393534080"/>
+        <c:axId val="393534640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="343330128"/>
+        <c:axId val="393534080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2037,7 +2032,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343324528"/>
+        <c:crossAx val="393534640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2045,7 +2040,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343324528"/>
+        <c:axId val="393534640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2096,7 +2091,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343330128"/>
+        <c:crossAx val="393534080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2110,7 +2105,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2217,6 +2211,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2568,11 +2563,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="397879168"/>
-        <c:axId val="397881408"/>
+        <c:axId val="393539680"/>
+        <c:axId val="393540240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="397879168"/>
+        <c:axId val="393539680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2615,7 +2610,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397881408"/>
+        <c:crossAx val="393540240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2623,7 +2618,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397881408"/>
+        <c:axId val="393540240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2674,7 +2669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397879168"/>
+        <c:crossAx val="393539680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2688,6 +2683,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2799,6 +2795,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3028,8 +3025,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="397880848"/>
-        <c:axId val="397879728"/>
+        <c:axId val="394720336"/>
+        <c:axId val="394720896"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -3117,7 +3114,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="397880848"/>
+        <c:axId val="394720336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3160,7 +3157,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397879728"/>
+        <c:crossAx val="394720896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3168,7 +3165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="397879728"/>
+        <c:axId val="394720896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3219,7 +3216,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="397880848"/>
+        <c:crossAx val="394720336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3233,6 +3230,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3447,11 +3445,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="413924144"/>
-        <c:axId val="413918544"/>
+        <c:axId val="394723696"/>
+        <c:axId val="394724256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="413924144"/>
+        <c:axId val="394723696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3494,7 +3492,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413918544"/>
+        <c:crossAx val="394724256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3502,7 +3500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="413918544"/>
+        <c:axId val="394724256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3553,7 +3551,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413924144"/>
+        <c:crossAx val="394723696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3743,11 +3741,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="413923024"/>
-        <c:axId val="413917984"/>
+        <c:axId val="394726496"/>
+        <c:axId val="394727056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="413923024"/>
+        <c:axId val="394726496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3790,7 +3788,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413917984"/>
+        <c:crossAx val="394727056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3798,7 +3796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="413917984"/>
+        <c:axId val="394727056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3849,7 +3847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="413923024"/>
+        <c:crossAx val="394726496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13450,7 +13448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
@@ -14879,7 +14877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>